<commit_message>
Add creating a new lead automation
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnr\eclipse-workspace\TestAutomationFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A220C6F8-2BA7-4C68-BDC4-967802E7D1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E55F8C3-80EC-4B43-B189-F4AC749D93EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{31A2FD57-B338-4984-B4AE-6125E793C50D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21390" activeTab="1" xr2:uid="{31A2FD57-B338-4984-B4AE-6125E793C50D}"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="LeadCreate" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -49,16 +49,25 @@
     <t>johnrickpogi23@gmail.com</t>
   </si>
   <si>
-    <t>johnrickgi23@gmail.com</t>
-  </si>
-  <si>
     <t>Testonly1234!</t>
   </si>
   <si>
-    <t>Testnly1234!</t>
-  </si>
-  <si>
-    <t>Testly1234!</t>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>SunnovaLLC</t>
+  </si>
+  <si>
+    <t>TestLast</t>
+  </si>
+  <si>
+    <t>TestFirst</t>
   </si>
 </sst>
 </file>
@@ -443,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9777CBC1-F347-4FD0-B07D-FE258A705496}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:F9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,41 +471,24 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{ACBCDAE9-32C0-4F45-A82C-01FB694EFFB6}"/>
-    <hyperlink ref="A3:A4" r:id="rId2" display="johnrickpogi23@gmail.com" xr:uid="{8B5CC736-13B7-4365-B609-9858AEF0A975}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{EB9A3C57-73A5-4994-BDC4-B7F57AEDA733}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D199DA74-CF8B-49B0-BD4C-457370F17602}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -504,13 +496,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D86313-C34E-46F3-8530-3B63CF22B3AD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6346ADED-8943-422F-97AE-72F4CEB17A96}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>